<commit_message>
General Fixes. Add new folder
</commit_message>
<xml_diff>
--- a/GB_Practics_API_Testing/Reg_&_auth_testing/Check-list.xlsx
+++ b/GB_Practics_API_Testing/Reg_&_auth_testing/Check-list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education\Video\Основы тестирования API (семинары)\Материалы\Practics\Reg_&amp;_auth_testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education\Practice\QA-Artifacts\GB_Practics_API_Testing\Reg_&amp;_auth_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49740D16-22D8-4DA4-BB7E-6A6ADAF25060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2C829B-669F-409F-963F-F27647632F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="59">
   <si>
     <t># номер</t>
   </si>
@@ -172,9 +172,6 @@
     <t>Образцы статуса</t>
   </si>
   <si>
-    <t>Ожидаемый статус - 200</t>
-  </si>
-  <si>
     <t>У нового пользователя отображается его имя, пароль и статус</t>
   </si>
   <si>
@@ -184,13 +181,22 @@
     <t>Данные значения отображаются в теле ответа</t>
   </si>
   <si>
-    <t>Ожидаемый статус - 400</t>
-  </si>
-  <si>
-    <t>Ожидаемый статус - 401</t>
-  </si>
-  <si>
     <t>Поле "birthDate" с датой соответвующей возрасту 101 год</t>
+  </si>
+  <si>
+    <t>Ожидаемый статус - 200/Фактический статус - 200</t>
+  </si>
+  <si>
+    <t>Ожидаемый статус - 400/Фактический статус - 200</t>
+  </si>
+  <si>
+    <t>Ожидаемый статус - 400/Фактический статус - 400</t>
+  </si>
+  <si>
+    <t>Ожидаемый статус - 200/Фактический статус - 400</t>
+  </si>
+  <si>
+    <t>Ожидаемый статус - 401/Фактический статус - 401</t>
   </si>
 </sst>
 </file>
@@ -569,7 +575,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -617,7 +623,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>4</v>
@@ -634,7 +640,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>5</v>
@@ -645,13 +651,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>6</v>
@@ -668,7 +674,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>7</v>
@@ -685,7 +691,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -699,7 +705,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -713,7 +719,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -727,7 +733,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -741,7 +747,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -755,7 +761,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -769,7 +775,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -783,7 +789,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -797,7 +803,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -811,7 +817,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -825,7 +831,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -839,7 +845,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -853,7 +859,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -867,7 +873,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -881,7 +887,7 @@
         <v>4</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -895,7 +901,7 @@
         <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -909,7 +915,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -923,7 +929,7 @@
         <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -937,7 +943,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -945,13 +951,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -965,7 +971,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -979,7 +985,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -993,7 +999,7 @@
         <v>5</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1007,7 +1013,7 @@
         <v>4</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1021,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1035,7 +1041,7 @@
         <v>5</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1049,7 +1055,7 @@
         <v>4</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1063,7 +1069,7 @@
         <v>4</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1077,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1091,7 +1097,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1105,7 +1111,7 @@
         <v>5</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1127,7 +1133,7 @@
         <v>4</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1141,7 +1147,7 @@
         <v>4</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1155,7 +1161,7 @@
         <v>4</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1169,7 +1175,7 @@
         <v>4</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1183,7 +1189,7 @@
         <v>4</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1197,7 +1203,7 @@
         <v>4</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>